<commit_message>
[FEAT](API/UI) Add schema-based config validation endpoint
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nzk\Documents\SaaS\json-automator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A7FA91-33FD-4300-A20F-9F3EC210D9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6660F2EC-52B4-4072-9B4B-A6F481B34DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>key</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>bool</t>
+  </si>
+  <si>
+    <t>random_key</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>string</t>
   </si>
 </sst>
 </file>
@@ -411,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -437,7 +446,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -465,7 +474,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -477,6 +486,20 @@
       </c>
       <c r="D4" s="2" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>